<commit_message>
export fotek, oprava ukladani catalogue
</commit_message>
<xml_diff>
--- a/TRIMAZKON/excel_testing_projekt_533.xlsx
+++ b/TRIMAZKON/excel_testing_projekt_533.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ST050 - foto" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ST250 - foto" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -239,6 +241,91 @@
       <rowOff>0</rowOff>
     </from>
     <ext cx="3114675" cy="1152525"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8229600" cy="9182100"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="11268075" cy="7439025"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="7734300" cy="9486900"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -611,7 +698,7 @@
       </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t>29.10.2024</t>
+          <t>31.10.2024</t>
         </is>
       </c>
     </row>
@@ -1258,7 +1345,7 @@
       </c>
       <c r="F25" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Alternativa: DLU-140W-HI
+          <t>
 </t>
         </is>
       </c>
@@ -1298,7 +1385,7 @@
       </c>
       <c r="F26" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Alternativa: 3Z4S-LE SV-3514H
+          <t>
 </t>
         </is>
       </c>
@@ -2409,4 +2496,42 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
práce na wrapování textboxů, downgrade xlsx - bylo to dobre vymyslene
</commit_message>
<xml_diff>
--- a/TRIMAZKON/excel_testing_projekt_533.xlsx
+++ b/TRIMAZKON/excel_testing_projekt_533.xlsx
@@ -241,91 +241,6 @@
       <rowOff>0</rowOff>
     </from>
     <ext cx="3114675" cy="1152525"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="8229600" cy="9182100"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>19</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="11268075" cy="7439025"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="7734300" cy="9486900"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -698,7 +613,7 @@
       </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t>07.11.2024</t>
+          <t>13.11.2024</t>
         </is>
       </c>
     </row>
@@ -734,7 +649,7 @@
       </c>
       <c r="J5" s="5" t="n"/>
     </row>
-    <row r="6" ht="180" customHeight="1">
+    <row r="6" ht="315" customHeight="1">
       <c r="A6" s="6" t="inlineStr">
         <is>
           <t>ST010</t>
@@ -753,13 +668,15 @@
       </c>
       <c r="D6" s="7" t="inlineStr">
         <is>
-          <t>Kabel: FZ-VS3 5M
-Kamera - popis: FH kamera, vysokorychlostní, 0.4 Mpixel, C  
-montáž, celková uzávěrka, monochromatická
-Kabel (FZ-VS3  
-5M): příslušenství kamerových systémů, FH a FZ, kabel ke  
-standardní kameře, 5m  
-http://industrial.omron.eu/en/search?q=G639</t>
+          <t xml:space="preserve">Kamera - popis: FH kamera, 
+vysokorychlostní, 0.4 Mpixel, C montáž, 
+celková uzávěrka, monochromatická
+Kabel (FZ-VS3 5M): příslušenství 
+kamerových systémů, FH a FZ, kabel ke 
+standardní kameře, 
+5m
+http://industrial.omron.eu/en/search?q=G639
+</t>
         </is>
       </c>
       <c r="E6" s="7" t="inlineStr">
@@ -767,7 +684,27 @@
           <t>3Z4S-LE SV-1614H</t>
         </is>
       </c>
-      <c r="F6" s="7" t="n"/>
+      <c r="F6" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternativa: 3Z4S-LE SV-10028H
+Objektiv - popis: Příslušenství pro 
+kamery, čočky, C montáž, pro kamery 
+FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, 
+FHV7H, ohnisková vzdálenost 12 mm, 
+nejmenší vzdálenost 100mm, světelnost 
+1,4 až 16, maximální kompatiblní CCD čip 
+2/3" nebo 1"
+Alternativní - popis: 
+Příslušenství pro kamery, čočky, C 
+montáž, pro kamery FZ-S_2M, FZ-S_5M3, 
+FH-S_05R, FH-S_X05, FHV7H, ohnisková 
+vzdálenost 75 mm, nejmenší vzdálenost 
+1200mm, světelnost 2,5 až zavřeno, 
+maximální kompatiblní CCD čip 2/3" nebo 
+1", revize 1
+</t>
+        </is>
+      </c>
       <c r="G6" s="8" t="inlineStr">
         <is>
           <t>FH-2051-20</t>
@@ -864,7 +801,12 @@
           <t>3Z4S-LE SV-2514H</t>
         </is>
       </c>
-      <c r="F9" s="7" t="n"/>
+      <c r="F9" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G9" s="8" t="inlineStr">
         <is>
           <t>FH-2051-20</t>
@@ -929,7 +871,12 @@
         </is>
       </c>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="7" t="n"/>
+      <c r="F11" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G11" s="7" t="n"/>
       <c r="H11" s="7" t="n"/>
       <c r="I11" s="7" t="n"/>
@@ -976,7 +923,12 @@
           <t>3Z4S-LE SV-2514H</t>
         </is>
       </c>
-      <c r="F13" s="7" t="n"/>
+      <c r="F13" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G13" s="8" t="inlineStr">
         <is>
           <t>FH-2051-20</t>
@@ -1071,7 +1023,12 @@
           <t>3Z4S-LE SV-5014H</t>
         </is>
       </c>
-      <c r="F16" s="7" t="n"/>
+      <c r="F16" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G16" s="8" t="inlineStr">
         <is>
           <t>FH-2051-20</t>
@@ -1137,7 +1094,7 @@
       <c r="I18" s="10" t="n"/>
       <c r="J18" s="10" t="n"/>
     </row>
-    <row r="19" ht="60" customHeight="1">
+    <row r="19" ht="135" customHeight="1">
       <c r="A19" s="6" t="inlineStr">
         <is>
           <t>ST070</t>
@@ -1166,7 +1123,12 @@
           <t>3Z4S-LE SV-3514H</t>
         </is>
       </c>
-      <c r="F19" s="7" t="n"/>
+      <c r="F19" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G19" s="7" t="inlineStr">
         <is>
           <t>FH-2051-10</t>
@@ -1196,7 +1158,7 @@
       <c r="C20" s="7" t="n"/>
       <c r="D20" s="7" t="n"/>
       <c r="E20" s="7" t="inlineStr"/>
-      <c r="F20" s="7" t="n"/>
+      <c r="F20" s="7" t="inlineStr"/>
       <c r="G20" s="7" t="n"/>
       <c r="H20" s="7" t="n"/>
       <c r="I20" s="7" t="inlineStr">
@@ -1217,7 +1179,7 @@
       <c r="C21" s="7" t="n"/>
       <c r="D21" s="7" t="n"/>
       <c r="E21" s="7" t="inlineStr"/>
-      <c r="F21" s="7" t="n"/>
+      <c r="F21" s="7" t="inlineStr"/>
       <c r="G21" s="7" t="n"/>
       <c r="H21" s="7" t="n"/>
       <c r="I21" s="7" t="inlineStr">
@@ -1232,7 +1194,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="30" customHeight="1">
+    <row r="22" ht="90" customHeight="1">
       <c r="A22" s="6" t="n"/>
       <c r="B22" s="7" t="n"/>
       <c r="C22" s="7" t="inlineStr">
@@ -1252,7 +1214,12 @@
           <t>3Z4S-LE SV-3514H</t>
         </is>
       </c>
-      <c r="F22" s="7" t="n"/>
+      <c r="F22" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G22" s="7" t="inlineStr">
         <is>
           <t>FH-2051-10</t>
@@ -1282,7 +1249,7 @@
       <c r="C23" s="7" t="n"/>
       <c r="D23" s="7" t="n"/>
       <c r="E23" s="7" t="inlineStr"/>
-      <c r="F23" s="7" t="n"/>
+      <c r="F23" s="7" t="inlineStr"/>
       <c r="G23" s="7" t="n"/>
       <c r="H23" s="7" t="n"/>
       <c r="I23" s="7" t="inlineStr">
@@ -1303,7 +1270,7 @@
       <c r="C24" s="7" t="n"/>
       <c r="D24" s="7" t="n"/>
       <c r="E24" s="7" t="inlineStr"/>
-      <c r="F24" s="7" t="n"/>
+      <c r="F24" s="7" t="inlineStr"/>
       <c r="G24" s="7" t="n"/>
       <c r="H24" s="7" t="n"/>
       <c r="I24" s="7" t="inlineStr">
@@ -1330,7 +1297,7 @@
       <c r="I25" s="10" t="n"/>
       <c r="J25" s="10" t="n"/>
     </row>
-    <row r="26" ht="60" customHeight="1">
+    <row r="26" ht="420" customHeight="1">
       <c r="A26" s="6" t="inlineStr">
         <is>
           <t>ST130</t>
@@ -1361,7 +1328,12 @@
           <t>3Z4S-LE SV-3514H</t>
         </is>
       </c>
-      <c r="F26" s="7" t="n"/>
+      <c r="F26" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G26" s="7" t="inlineStr">
         <is>
           <t>FH-2051-10</t>
@@ -1395,7 +1367,12 @@
           <t>3Z4S-LE SV-5014H</t>
         </is>
       </c>
-      <c r="F27" s="7" t="n"/>
+      <c r="F27" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G27" s="7" t="n"/>
       <c r="H27" s="7" t="n"/>
       <c r="I27" s="7" t="inlineStr">
@@ -1416,7 +1393,7 @@
       <c r="C28" s="7" t="n"/>
       <c r="D28" s="7" t="n"/>
       <c r="E28" s="7" t="inlineStr"/>
-      <c r="F28" s="7" t="n"/>
+      <c r="F28" s="7" t="inlineStr"/>
       <c r="G28" s="7" t="n"/>
       <c r="H28" s="7" t="n"/>
       <c r="I28" s="7" t="inlineStr">
@@ -1431,7 +1408,7 @@
         </is>
       </c>
     </row>
-    <row r="29" ht="30" customHeight="1">
+    <row r="29" ht="90" customHeight="1">
       <c r="A29" s="6" t="n"/>
       <c r="B29" s="7" t="n"/>
       <c r="C29" s="7" t="inlineStr">
@@ -1441,7 +1418,11 @@
       </c>
       <c r="D29" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Svìtlo: SP-27IR-850
+          <t xml:space="preserve">Kamera - popis: Kamera FH 3D, FOV 
+400x300x200 mm, WD 500 mm, 24 V
+Kabel 
+(FZ-VSBX 5M): Ultra bend resistant 
+camera cable, 5 m
 </t>
         </is>
       </c>
@@ -1450,7 +1431,12 @@
           <t>3Z4S-LE SV-5014H</t>
         </is>
       </c>
-      <c r="F29" s="7" t="n"/>
+      <c r="F29" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G29" s="7" t="inlineStr">
         <is>
           <t>FH-2051-10</t>
@@ -1484,7 +1470,12 @@
           <t>3Z4S-LE SV-2514H</t>
         </is>
       </c>
-      <c r="F30" s="7" t="n"/>
+      <c r="F30" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G30" s="7" t="n"/>
       <c r="H30" s="7" t="n"/>
       <c r="I30" s="7" t="inlineStr">
@@ -1509,7 +1500,12 @@
           <t>LA-70B</t>
         </is>
       </c>
-      <c r="F31" s="7" t="n"/>
+      <c r="F31" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G31" s="7" t="n"/>
       <c r="H31" s="7" t="n"/>
       <c r="I31" s="7" t="inlineStr">
@@ -1534,7 +1530,13 @@
           <t>LA-70B</t>
         </is>
       </c>
-      <c r="F32" s="7" t="n"/>
+      <c r="F32" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternativa: FL-MD90MC
+sfffffffffffin spection_description sfffffffffffin spection_description sfffffffffffin spection_description sfffffffffffin spection_description sfffffffffffin spection_description sfffffffffffin spection_description sfffffffffffin spection_description sfffffffffffin spection_description sfffffffffffin spection_description sfffffffffffin spection_description sfffffffffffin spection_description sfffffffffffin spection_description sfffffffffffin spection_description sfffffffffffin spection_description sfffffffffffin spection_description sfffffffffffin spection_description 
+</t>
+        </is>
+      </c>
       <c r="G32" s="7" t="n"/>
       <c r="H32" s="7" t="n"/>
       <c r="I32" s="7" t="n"/>
@@ -1550,7 +1552,12 @@
           <t>3Z4S-LE SV-2514H</t>
         </is>
       </c>
-      <c r="F33" s="7" t="n"/>
+      <c r="F33" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G33" s="7" t="n"/>
       <c r="H33" s="7" t="n"/>
       <c r="I33" s="7" t="n"/>
@@ -1566,7 +1573,18 @@
           <t>3Z4S-LE SV-1614H</t>
         </is>
       </c>
-      <c r="F34" s="7" t="n"/>
+      <c r="F34" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Objektiv - popis: Příslušenství pro 
+kamery, čočky, C montáž, pro kamery 
+FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, 
+FHV7H, ohnisková vzdálenost 12 mm, 
+nejmenší vzdálenost 100mm, světelnost 
+1,4 až 16, maximální kompatiblní CCD čip 
+2/3" nebo 1"
+</t>
+        </is>
+      </c>
       <c r="G34" s="7" t="n"/>
       <c r="H34" s="7" t="n"/>
       <c r="I34" s="7" t="n"/>
@@ -1591,7 +1609,12 @@
           <t>T030/9,1-85-V-BW</t>
         </is>
       </c>
-      <c r="F35" s="7" t="n"/>
+      <c r="F35" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G35" s="7" t="n"/>
       <c r="H35" s="7" t="n"/>
       <c r="I35" s="7" t="n"/>
@@ -1609,7 +1632,7 @@
       <c r="I36" s="10" t="n"/>
       <c r="J36" s="10" t="n"/>
     </row>
-    <row r="37">
+    <row r="37" ht="30" customHeight="1">
       <c r="A37" s="6" t="inlineStr">
         <is>
           <t>PRE:</t>
@@ -1642,7 +1665,7 @@
       <c r="I38" s="10" t="n"/>
       <c r="J38" s="10" t="n"/>
     </row>
-    <row r="39" ht="30" customHeight="1">
+    <row r="39" ht="120" customHeight="1">
       <c r="A39" s="6" t="inlineStr">
         <is>
           <t>ST250</t>
@@ -1671,7 +1694,12 @@
           <t>TO42/21.4-120-V-BW</t>
         </is>
       </c>
-      <c r="F39" s="7" t="n"/>
+      <c r="F39" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Telecentrika
+</t>
+        </is>
+      </c>
       <c r="G39" s="12" t="inlineStr">
         <is>
           <t>FH-2051-10</t>
@@ -1705,7 +1733,12 @@
           <t>3Z4S-LE SV-5014H</t>
         </is>
       </c>
-      <c r="F40" s="7" t="n"/>
+      <c r="F40" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G40" s="7" t="n"/>
       <c r="H40" s="7" t="n"/>
       <c r="I40" s="7" t="inlineStr">
@@ -1730,7 +1763,12 @@
           <t>LA-70W</t>
         </is>
       </c>
-      <c r="F41" s="7" t="n"/>
+      <c r="F41" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G41" s="7" t="n"/>
       <c r="H41" s="7" t="n"/>
       <c r="I41" s="7" t="inlineStr">
@@ -1755,7 +1793,12 @@
           <t>BL-50W-4S</t>
         </is>
       </c>
-      <c r="F42" s="7" t="n"/>
+      <c r="F42" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G42" s="7" t="n"/>
       <c r="H42" s="7" t="n"/>
       <c r="I42" s="7" t="n"/>
@@ -1773,7 +1816,7 @@
       <c r="I43" s="10" t="n"/>
       <c r="J43" s="10" t="n"/>
     </row>
-    <row r="44" ht="30" customHeight="1">
+    <row r="44" ht="90" customHeight="1">
       <c r="A44" s="6" t="inlineStr">
         <is>
           <t>ST270</t>
@@ -1802,7 +1845,12 @@
           <t>TO42/16.0-120-V-BW</t>
         </is>
       </c>
-      <c r="F44" s="7" t="n"/>
+      <c r="F44" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Telecentrika 
+</t>
+        </is>
+      </c>
       <c r="G44" s="12" t="inlineStr">
         <is>
           <t>FH-2051-10</t>
@@ -1832,7 +1880,7 @@
       <c r="C45" s="7" t="n"/>
       <c r="D45" s="7" t="n"/>
       <c r="E45" s="7" t="inlineStr"/>
-      <c r="F45" s="7" t="n"/>
+      <c r="F45" s="7" t="inlineStr"/>
       <c r="G45" s="7" t="n"/>
       <c r="H45" s="7" t="n"/>
       <c r="I45" s="7" t="inlineStr">
@@ -1853,7 +1901,7 @@
       <c r="C46" s="7" t="n"/>
       <c r="D46" s="7" t="n"/>
       <c r="E46" s="7" t="inlineStr"/>
-      <c r="F46" s="7" t="n"/>
+      <c r="F46" s="7" t="inlineStr"/>
       <c r="G46" s="7" t="n"/>
       <c r="H46" s="7" t="n"/>
       <c r="I46" s="7" t="inlineStr">
@@ -1880,7 +1928,7 @@
       <c r="I47" s="10" t="n"/>
       <c r="J47" s="10" t="n"/>
     </row>
-    <row r="48" ht="30" customHeight="1">
+    <row r="48" ht="90" customHeight="1">
       <c r="A48" s="6" t="inlineStr">
         <is>
           <t>ST290</t>
@@ -1909,7 +1957,12 @@
           <t>TO42/16.0-120-V-BW</t>
         </is>
       </c>
-      <c r="F48" s="7" t="n"/>
+      <c r="F48" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G48" s="12" t="inlineStr">
         <is>
           <t>FH-2051-10</t>
@@ -1939,7 +1992,7 @@
       <c r="C49" s="7" t="n"/>
       <c r="D49" s="7" t="n"/>
       <c r="E49" s="7" t="inlineStr"/>
-      <c r="F49" s="7" t="n"/>
+      <c r="F49" s="7" t="inlineStr"/>
       <c r="G49" s="7" t="n"/>
       <c r="H49" s="7" t="n"/>
       <c r="I49" s="7" t="inlineStr">
@@ -1960,7 +2013,7 @@
       <c r="C50" s="7" t="n"/>
       <c r="D50" s="7" t="n"/>
       <c r="E50" s="7" t="inlineStr"/>
-      <c r="F50" s="7" t="n"/>
+      <c r="F50" s="7" t="inlineStr"/>
       <c r="G50" s="7" t="n"/>
       <c r="H50" s="7" t="n"/>
       <c r="I50" s="7" t="inlineStr">
@@ -1987,7 +2040,7 @@
       <c r="I51" s="10" t="n"/>
       <c r="J51" s="10" t="n"/>
     </row>
-    <row r="52" ht="30" customHeight="1">
+    <row r="52" ht="90" customHeight="1">
       <c r="A52" s="6" t="inlineStr">
         <is>
           <t>ST310</t>
@@ -2015,7 +2068,12 @@
           <t>TO42/16.0-120-V-BW</t>
         </is>
       </c>
-      <c r="F52" s="7" t="n"/>
+      <c r="F52" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Telecentrika
+</t>
+        </is>
+      </c>
       <c r="G52" s="13" t="inlineStr">
         <is>
           <t>FH-2051-20</t>
@@ -2045,7 +2103,7 @@
       <c r="C53" s="7" t="n"/>
       <c r="D53" s="7" t="n"/>
       <c r="E53" s="7" t="inlineStr"/>
-      <c r="F53" s="7" t="n"/>
+      <c r="F53" s="7" t="inlineStr"/>
       <c r="G53" s="7" t="n"/>
       <c r="H53" s="7" t="n"/>
       <c r="I53" s="7" t="inlineStr">
@@ -2066,7 +2124,7 @@
       <c r="C54" s="7" t="n"/>
       <c r="D54" s="7" t="n"/>
       <c r="E54" s="7" t="inlineStr"/>
-      <c r="F54" s="7" t="n"/>
+      <c r="F54" s="7" t="inlineStr"/>
       <c r="G54" s="7" t="n"/>
       <c r="H54" s="7" t="n"/>
       <c r="I54" s="7" t="inlineStr">
@@ -2093,7 +2151,7 @@
       <c r="I55" s="10" t="n"/>
       <c r="J55" s="10" t="n"/>
     </row>
-    <row r="56" ht="120" customHeight="1">
+    <row r="56" ht="135" customHeight="1">
       <c r="A56" s="6" t="inlineStr">
         <is>
           <t>ST360</t>
@@ -2129,7 +2187,12 @@
           <t>3Z4S-LE SV-3514H</t>
         </is>
       </c>
-      <c r="F56" s="7" t="n"/>
+      <c r="F56" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G56" s="13" t="inlineStr">
         <is>
           <t>FH-2051-20</t>
@@ -2159,7 +2222,7 @@
       <c r="C57" s="7" t="n"/>
       <c r="D57" s="7" t="n"/>
       <c r="E57" s="7" t="inlineStr"/>
-      <c r="F57" s="7" t="n"/>
+      <c r="F57" s="7" t="inlineStr"/>
       <c r="G57" s="7" t="n"/>
       <c r="H57" s="7" t="n"/>
       <c r="I57" s="7" t="inlineStr">
@@ -2180,7 +2243,7 @@
       <c r="C58" s="7" t="n"/>
       <c r="D58" s="7" t="n"/>
       <c r="E58" s="7" t="inlineStr"/>
-      <c r="F58" s="7" t="n"/>
+      <c r="F58" s="7" t="inlineStr"/>
       <c r="G58" s="7" t="n"/>
       <c r="H58" s="7" t="n"/>
       <c r="I58" s="7" t="inlineStr">
@@ -2207,7 +2270,7 @@
       <c r="I59" s="10" t="n"/>
       <c r="J59" s="10" t="n"/>
     </row>
-    <row r="60" ht="45" customHeight="1">
+    <row r="60" ht="120" customHeight="1">
       <c r="A60" s="6" t="inlineStr">
         <is>
           <t>ST410</t>
@@ -2236,7 +2299,12 @@
           <t>3Z4S-LE SV-3514H</t>
         </is>
       </c>
-      <c r="F60" s="7" t="n"/>
+      <c r="F60" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G60" s="13" t="inlineStr">
         <is>
           <t>FH-2051-20</t>
@@ -2270,7 +2338,12 @@
           <t>BL-50W-4S</t>
         </is>
       </c>
-      <c r="F61" s="7" t="n"/>
+      <c r="F61" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G61" s="7" t="n"/>
       <c r="H61" s="7" t="n"/>
       <c r="I61" s="7" t="inlineStr">
@@ -2291,7 +2364,12 @@
       <c r="C62" s="7" t="n"/>
       <c r="D62" s="7" t="n"/>
       <c r="E62" s="7" t="inlineStr"/>
-      <c r="F62" s="7" t="n"/>
+      <c r="F62" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">5465
+</t>
+        </is>
+      </c>
       <c r="G62" s="7" t="n"/>
       <c r="H62" s="7" t="n"/>
       <c r="I62" s="7" t="inlineStr">
@@ -2321,7 +2399,12 @@
         </is>
       </c>
       <c r="E63" s="7" t="inlineStr"/>
-      <c r="F63" s="7" t="n"/>
+      <c r="F63" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G63" s="7" t="n"/>
       <c r="H63" s="7" t="n"/>
       <c r="I63" s="7" t="n"/>
@@ -2339,7 +2422,7 @@
       <c r="I64" s="10" t="n"/>
       <c r="J64" s="10" t="n"/>
     </row>
-    <row r="65" ht="30" customHeight="1">
+    <row r="65" ht="90" customHeight="1">
       <c r="A65" s="6" t="inlineStr">
         <is>
           <t>ST395</t>
@@ -2363,7 +2446,12 @@
         </is>
       </c>
       <c r="E65" s="7" t="inlineStr"/>
-      <c r="F65" s="7" t="n"/>
+      <c r="F65" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G65" s="14" t="inlineStr">
         <is>
           <t>FH-2051-10</t>
@@ -2378,7 +2466,7 @@
       <c r="I65" s="7" t="inlineStr"/>
       <c r="J65" s="7" t="inlineStr"/>
     </row>
-    <row r="66" ht="30" customHeight="1">
+    <row r="66" ht="90" customHeight="1">
       <c r="A66" s="6" t="n"/>
       <c r="B66" s="7" t="n"/>
       <c r="C66" s="7" t="inlineStr">
@@ -2393,7 +2481,12 @@
         </is>
       </c>
       <c r="E66" s="7" t="inlineStr"/>
-      <c r="F66" s="7" t="n"/>
+      <c r="F66" s="7" t="inlineStr">
+        <is>
+          <t>
+</t>
+        </is>
+      </c>
       <c r="G66" s="14" t="inlineStr">
         <is>
           <t>FH-2051-10</t>
@@ -2528,7 +2621,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2542,12 +2635,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2561,6 +2653,5 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dokoncene funkcni wrapovani textboxů, přidaná kontextová nabídka na každý widget
</commit_message>
<xml_diff>
--- a/TRIMAZKON/excel_testing_projekt_533.xlsx
+++ b/TRIMAZKON/excel_testing_projekt_533.xlsx
@@ -241,6 +241,91 @@
       <rowOff>0</rowOff>
     </from>
     <ext cx="3114675" cy="1152525"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="8229600" cy="9182100"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="11268075" cy="7439025"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="7734300" cy="9486900"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -613,7 +698,7 @@
       </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t>13.11.2024</t>
+          <t>14.11.2024</t>
         </is>
       </c>
     </row>
@@ -649,7 +734,7 @@
       </c>
       <c r="J5" s="5" t="n"/>
     </row>
-    <row r="6" ht="315" customHeight="1">
+    <row r="6" ht="285" customHeight="1">
       <c r="A6" s="6" t="inlineStr">
         <is>
           <t>ST010</t>
@@ -657,8 +742,9 @@
       </c>
       <c r="B6" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">kontrola tvaru/modelu senzoru (pohled ze strany senzoru) jsou dva modely – vzdálenost  
-</t>
+          <t>kontrola tvaru/modelu senzoru (pohled 
+ze strany senzoru) jsou dva modely – 
+vzdálenost</t>
         </is>
       </c>
       <c r="C6" s="7" t="inlineStr">
@@ -668,15 +754,14 @@
       </c>
       <c r="D6" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kamera - popis: FH kamera, 
+          <t xml:space="preserve">Kamera - popis: FH kamera,
 vysokorychlostní, 0.4 Mpixel, C montáž, 
 celková uzávěrka, monochromatická
-Kabel (FZ-VS3 5M): příslušenství 
+Kabel (FZ-VS3 5M): příslušenství
 kamerových systémů, FH a FZ, kabel ke 
-standardní kameře, 
+standardní kameře,
 5m
-http://industrial.omron.eu/en/search?q=G639
-</t>
+http://industrial.omron.eu/en/search?q=G639 </t>
         </is>
       </c>
       <c r="E6" s="7" t="inlineStr">
@@ -686,23 +771,22 @@
       </c>
       <c r="F6" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Alternativa: 3Z4S-LE SV-10028H
-Objektiv - popis: Příslušenství pro 
-kamery, čočky, C montáž, pro kamery 
+          <t>Alternativa: 3Z4S-LE SV-10028H
+Objektiv - popis: Příslušenství pro
+kamery, čočky, C montáž, pro kamery
 FZ-S_2M, FZ-S_5M3, FH-S_05R, FH-S_X05, 
-FHV7H, ohnisková vzdálenost 12 mm, 
+FHV7H, ohnisková vzdálenost 12 mm,
 nejmenší vzdálenost 100mm, světelnost 
 1,4 až 16, maximální kompatiblní CCD čip 
 2/3" nebo 1"
-Alternativní - popis: 
-Příslušenství pro kamery, čočky, C 
+Alternativní - popis:
+Příslušenství pro kamery, čočky, C
 montáž, pro kamery FZ-S_2M, FZ-S_5M3, 
 FH-S_05R, FH-S_X05, FHV7H, ohnisková 
 vzdálenost 75 mm, nejmenší vzdálenost 
-1200mm, světelnost 2,5 až zavřeno, 
+1200mm, světelnost 2,5 až zavřeno,
 maximální kompatiblní CCD čip 2/3" nebo 
-1", revize 1
-</t>
+1", revize 1</t>
         </is>
       </c>
       <c r="G6" s="8" t="inlineStr">
@@ -743,8 +827,8 @@
       <c r="B7" s="7" t="n"/>
       <c r="C7" s="7" t="n"/>
       <c r="D7" s="7" t="n"/>
-      <c r="E7" s="7" t="n"/>
-      <c r="F7" s="7" t="n"/>
+      <c r="E7" s="7" t="inlineStr"/>
+      <c r="F7" s="7" t="inlineStr"/>
       <c r="G7" s="7" t="n"/>
       <c r="H7" s="7" t="n"/>
       <c r="I7" s="7" t="inlineStr">
@@ -778,9 +862,10 @@
       </c>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Guma – ověřit barvu (bude modrá) původní je oranžová 
-Pozice gumy na ploše cca 50x50 mm - kamera zespodu pod sklem 
-</t>
+          <t>Guma – ověřit barvu (bude modrá) původní 
+je oranžová
+Pozice gumy na ploše cca 50x50
+mm - kamera zespodu pod sklem</t>
         </is>
       </c>
       <c r="C9" s="7" t="inlineStr">
@@ -790,10 +875,9 @@
       </c>
       <c r="D9" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">5Mpx kamera
-Low-angle světlo (testováno s LA-120W)
-Svìtlo: LA-120W
-</t>
+          <t>5Mpx kamera
+Low-angle světlo (testováno s LA-120W) 
+Svìtlo: LA-120W</t>
         </is>
       </c>
       <c r="E9" s="7" t="inlineStr">
@@ -801,12 +885,7 @@
           <t>3Z4S-LE SV-2514H</t>
         </is>
       </c>
-      <c r="F9" s="7" t="inlineStr">
-        <is>
-          <t>
-</t>
-        </is>
-      </c>
+      <c r="F9" s="7" t="inlineStr"/>
       <c r="G9" s="8" t="inlineStr">
         <is>
           <t>FH-2051-20</t>
@@ -845,8 +924,8 @@
       <c r="B10" s="7" t="n"/>
       <c r="C10" s="7" t="n"/>
       <c r="D10" s="7" t="n"/>
-      <c r="E10" s="7" t="n"/>
-      <c r="F10" s="7" t="n"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
       <c r="G10" s="7" t="n"/>
       <c r="H10" s="7" t="n"/>
       <c r="I10" s="7" t="inlineStr">
@@ -864,19 +943,9 @@
       <c r="A11" s="6" t="n"/>
       <c r="B11" s="7" t="n"/>
       <c r="C11" s="7" t="inlineStr"/>
-      <c r="D11" s="7" t="inlineStr">
-        <is>
-          <t>
-</t>
-        </is>
-      </c>
+      <c r="D11" s="7" t="inlineStr"/>
       <c r="E11" s="7" t="inlineStr"/>
-      <c r="F11" s="7" t="inlineStr">
-        <is>
-          <t>
-</t>
-        </is>
-      </c>
+      <c r="F11" s="7" t="inlineStr"/>
       <c r="G11" s="7" t="n"/>
       <c r="H11" s="7" t="n"/>
       <c r="I11" s="7" t="n"/>
@@ -902,8 +971,8 @@
       </c>
       <c r="B13" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kontrola barvy senzoru – chtějí dva kusy najednou… 
-</t>
+          <t>Kontrola barvy senzoru – chtějí dva kusy 
+najednou…</t>
         </is>
       </c>
       <c r="C13" s="7" t="inlineStr">
@@ -913,9 +982,8 @@
       </c>
       <c r="D13" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Svìtlo: DLU-140W-HI
-- v modelu
-</t>
+          <t>Svìtlo: DLU-140W-HI
+- v modelu</t>
         </is>
       </c>
       <c r="E13" s="7" t="inlineStr">
@@ -923,12 +991,7 @@
           <t>3Z4S-LE SV-2514H</t>
         </is>
       </c>
-      <c r="F13" s="7" t="inlineStr">
-        <is>
-          <t>
-</t>
-        </is>
-      </c>
+      <c r="F13" s="7" t="inlineStr"/>
       <c r="G13" s="8" t="inlineStr">
         <is>
           <t>FH-2051-20</t>
@@ -967,8 +1030,8 @@
       <c r="B14" s="7" t="n"/>
       <c r="C14" s="7" t="n"/>
       <c r="D14" s="7" t="n"/>
-      <c r="E14" s="7" t="n"/>
-      <c r="F14" s="7" t="n"/>
+      <c r="E14" s="7" t="inlineStr"/>
+      <c r="F14" s="7" t="inlineStr"/>
       <c r="G14" s="7" t="n"/>
       <c r="H14" s="7" t="n"/>
       <c r="I14" s="7" t="inlineStr">
@@ -1067,8 +1130,8 @@
       <c r="B17" s="7" t="n"/>
       <c r="C17" s="7" t="n"/>
       <c r="D17" s="7" t="n"/>
-      <c r="E17" s="7" t="n"/>
-      <c r="F17" s="7" t="n"/>
+      <c r="E17" s="7" t="inlineStr"/>
+      <c r="F17" s="7" t="inlineStr"/>
       <c r="G17" s="7" t="n"/>
       <c r="H17" s="7" t="n"/>
       <c r="I17" s="7" t="inlineStr">
@@ -2514,7 +2577,7 @@
       <c r="J67" s="15" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="99">
+  <mergeCells count="91">
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="C48:C50"/>
     <mergeCell ref="A16:A17"/>
@@ -2528,7 +2591,6 @@
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="F13:F14"/>
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="H13:H14"/>
     <mergeCell ref="C44:C46"/>
@@ -2537,10 +2599,8 @@
     <mergeCell ref="A39:A42"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="A19:A24"/>
-    <mergeCell ref="F16:F17"/>
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="D56:D58"/>
-    <mergeCell ref="E13:E14"/>
     <mergeCell ref="G39:G42"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="G13:G14"/>
@@ -2556,7 +2616,6 @@
     <mergeCell ref="H44:H46"/>
     <mergeCell ref="B60:B63"/>
     <mergeCell ref="G48:G50"/>
-    <mergeCell ref="F9:F10"/>
     <mergeCell ref="C26:C28"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="B48:B50"/>
@@ -2580,7 +2639,6 @@
     <mergeCell ref="B52:B54"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="D52:D54"/>
-    <mergeCell ref="E16:E17"/>
     <mergeCell ref="B19:B24"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="G29:G34"/>
@@ -2589,7 +2647,6 @@
     <mergeCell ref="B44:B46"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="C60:C62"/>
-    <mergeCell ref="F6:F7"/>
     <mergeCell ref="A56:A58"/>
     <mergeCell ref="C56:C58"/>
     <mergeCell ref="H22:H24"/>
@@ -2597,11 +2654,9 @@
     <mergeCell ref="I41:I42"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="G44:G46"/>
-    <mergeCell ref="E9:E10"/>
     <mergeCell ref="H48:H50"/>
     <mergeCell ref="C19:C21"/>
     <mergeCell ref="G52:G54"/>
-    <mergeCell ref="E6:E7"/>
     <mergeCell ref="B56:B58"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="B1:C3"/>
@@ -2621,7 +2676,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2635,11 +2690,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -2653,5 +2709,6 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>